<commit_message>
ajout modal visu politic
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -438,7 +438,7 @@
         <v>76210</v>
       </c>
       <c r="G2" t="str">
-        <v>114</v>
+        <v>76114</v>
       </c>
     </row>
     <row r="3">
@@ -461,7 +461,7 @@
         <v>35000</v>
       </c>
       <c r="G3" t="str">
-        <v>238</v>
+        <v>35238</v>
       </c>
       <c r="H3" t="str">
         <v>https://www.ouest-france.fr/bretagne/rennes-35000/portrait-qui-est-carole-gandon-la-marcheuse-qui-veut-gagner-la-mairie-de-rennes-6322212</v>
@@ -487,7 +487,7 @@
         <v>35510</v>
       </c>
       <c r="G4" t="str">
-        <v>051</v>
+        <v>35051</v>
       </c>
     </row>
     <row r="5">
@@ -510,7 +510,7 @@
         <v>22300</v>
       </c>
       <c r="G5" t="str">
-        <v>113</v>
+        <v>22113</v>
       </c>
     </row>
     <row r="6">
@@ -533,7 +533,7 @@
         <v>29900</v>
       </c>
       <c r="G6" t="str">
-        <v>039</v>
+        <v>29039</v>
       </c>
     </row>
     <row r="7">
@@ -556,7 +556,7 @@
         <v>56600</v>
       </c>
       <c r="G7" t="str">
-        <v>098</v>
+        <v>56098</v>
       </c>
     </row>
     <row r="8">
@@ -579,7 +579,7 @@
         <v>35170</v>
       </c>
       <c r="G8" t="str">
-        <v>047</v>
+        <v>35047</v>
       </c>
     </row>
     <row r="9">
@@ -602,7 +602,7 @@
         <v>29470</v>
       </c>
       <c r="G9" t="str">
-        <v>189</v>
+        <v>29189</v>
       </c>
     </row>
     <row r="10">
@@ -625,7 +625,7 @@
         <v>56400</v>
       </c>
       <c r="G10" t="str">
-        <v>007</v>
+        <v>56007</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -654,7 +654,7 @@
         <v>56100</v>
       </c>
       <c r="G11" t="str">
-        <v>121</v>
+        <v>56121</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>29600</v>
       </c>
       <c r="G12" t="str">
-        <v>151</v>
+        <v>29151</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -712,7 +712,7 @@
         <v>29490</v>
       </c>
       <c r="G13" t="str">
-        <v>075</v>
+        <v>29075</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -741,7 +741,7 @@
         <v>56300</v>
       </c>
       <c r="G14" t="str">
-        <v>178</v>
+        <v>56178</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>35800</v>
       </c>
       <c r="G15" t="str">
-        <v>093</v>
+        <v>35093</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>35136</v>
       </c>
       <c r="G16" t="str">
-        <v>281</v>
+        <v>35281</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -828,7 +828,7 @@
         <v>29280</v>
       </c>
       <c r="G17" t="str">
-        <v>212</v>
+        <v>29212</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -857,7 +857,7 @@
         <v>29400</v>
       </c>
       <c r="G18" t="str">
-        <v>105</v>
+        <v>29105</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -886,7 +886,7 @@
         <v>22400</v>
       </c>
       <c r="G19" t="str">
-        <v>093</v>
+        <v>22093</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -915,7 +915,7 @@
         <v>29000</v>
       </c>
       <c r="G20" t="str">
-        <v>232</v>
+        <v>29232</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -973,7 +973,7 @@
         <v>29200</v>
       </c>
       <c r="G22" t="str">
-        <v>019</v>
+        <v>29019</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>56000</v>
       </c>
       <c r="G23" t="str">
-        <v>260</v>
+        <v>56260</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>76230</v>
       </c>
       <c r="G24" t="str">
-        <v>108</v>
+        <v>76108</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         <v>61000</v>
       </c>
       <c r="G25" t="str">
-        <v>001</v>
+        <v>61001</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1089,7 +1089,7 @@
         <v>76190</v>
       </c>
       <c r="G26" t="str">
-        <v>758</v>
+        <v>76758</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1147,7 +1147,7 @@
         <v>76130</v>
       </c>
       <c r="G28" t="str">
-        <v>451</v>
+        <v>76451</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1176,7 +1176,7 @@
         <v>76000</v>
       </c>
       <c r="G29" t="str">
-        <v>540</v>
+        <v>76540</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1234,7 +1234,7 @@
         <v>76380</v>
       </c>
       <c r="G31" t="str">
-        <v>157</v>
+        <v>76157</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>14500</v>
       </c>
       <c r="G32" t="str">
-        <v>762</v>
+        <v>14762</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1292,7 +1292,7 @@
         <v>50100</v>
       </c>
       <c r="G33" t="str">
-        <v>129</v>
+        <v>50129</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1321,7 +1321,7 @@
         <v>13200</v>
       </c>
       <c r="G34" t="str">
-        <v>004</v>
+        <v>13004</v>
       </c>
     </row>
     <row r="35">
@@ -1341,7 +1341,7 @@
         <v>13410</v>
       </c>
       <c r="G35" t="str">
-        <v>050</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="36">
@@ -1361,7 +1361,7 @@
         <v>13400</v>
       </c>
       <c r="G36" t="str">
-        <v>005</v>
+        <v>13005</v>
       </c>
     </row>
     <row r="37">
@@ -1381,7 +1381,7 @@
         <v>13400</v>
       </c>
       <c r="G37" t="str">
-        <v>005</v>
+        <v>13005</v>
       </c>
     </row>
     <row r="38">
@@ -1401,7 +1401,7 @@
         <v>13500</v>
       </c>
       <c r="G38" t="str">
-        <v>056</v>
+        <v>13056</v>
       </c>
     </row>
     <row r="39">
@@ -1421,7 +1421,7 @@
         <v>13500</v>
       </c>
       <c r="G39" t="str">
-        <v>056</v>
+        <v>13056</v>
       </c>
     </row>
     <row r="40">
@@ -1441,7 +1441,7 @@
         <v>13800</v>
       </c>
       <c r="G40" t="str">
-        <v>047</v>
+        <v>13047</v>
       </c>
     </row>
     <row r="41">
@@ -1461,7 +1461,7 @@
         <v>13480</v>
       </c>
       <c r="G41" t="str">
-        <v>019</v>
+        <v>13019</v>
       </c>
     </row>
     <row r="42">
@@ -1484,7 +1484,7 @@
         <v>13210</v>
       </c>
       <c r="G42" t="str">
-        <v>100</v>
+        <v>13100</v>
       </c>
     </row>
     <row r="43">
@@ -1504,7 +1504,7 @@
         <v>13530</v>
       </c>
       <c r="G43" t="str">
-        <v>110</v>
+        <v>13110</v>
       </c>
     </row>
     <row r="44">
@@ -1553,7 +1553,7 @@
         <v>83200</v>
       </c>
       <c r="G45" t="str">
-        <v>137</v>
+        <v>83137</v>
       </c>
     </row>
     <row r="46">
@@ -1573,7 +1573,7 @@
         <v>83130</v>
       </c>
       <c r="G46" t="str">
-        <v>092</v>
+        <v>04092</v>
       </c>
     </row>
     <row r="47">
@@ -1593,7 +1593,7 @@
         <v>83530</v>
       </c>
       <c r="G47" t="str">
-        <v>493</v>
+        <v>24493</v>
       </c>
     </row>
     <row r="48">
@@ -1613,7 +1613,7 @@
         <v>83380</v>
       </c>
       <c r="G48" t="str">
-        <v>107</v>
+        <v>83107</v>
       </c>
     </row>
     <row r="49">
@@ -1636,7 +1636,7 @@
         <v>83400</v>
       </c>
       <c r="G49" t="str">
-        <v>069</v>
+        <v>83069</v>
       </c>
     </row>
     <row r="50">
@@ -1656,7 +1656,7 @@
         <v>83320</v>
       </c>
       <c r="G50" t="str">
-        <v>034</v>
+        <v>83034</v>
       </c>
     </row>
     <row r="51">
@@ -1676,7 +1676,7 @@
         <v>83370</v>
       </c>
       <c r="G51" t="str">
-        <v>061</v>
+        <v>83061</v>
       </c>
     </row>
     <row r="52">
@@ -1719,7 +1719,7 @@
         <v>49000</v>
       </c>
       <c r="G53" t="str">
-        <v>007</v>
+        <v>49007</v>
       </c>
       <c r="H53" t="str">
         <v>https://twitter.com/LaREMpourTous/status/1214107975482249217?s=20</v>
@@ -1748,7 +1748,7 @@
         <v>70000</v>
       </c>
       <c r="G54" t="str">
-        <v>550</v>
+        <v>70550</v>
       </c>
       <c r="H54" t="str">
         <v>https://twitter.com/LaREMpourTous/status/1213719728298110977?s=20</v>
@@ -1774,7 +1774,7 @@
         <v>44500</v>
       </c>
       <c r="G55" t="str">
-        <v>055</v>
+        <v>44055</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -1803,7 +1803,7 @@
         <v>49300</v>
       </c>
       <c r="G56" t="str">
-        <v>099</v>
+        <v>49099</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -1832,7 +1832,7 @@
         <v>85100</v>
       </c>
       <c r="G57" t="str">
-        <v>194</v>
+        <v>85194</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -1861,7 +1861,7 @@
         <v>44220</v>
       </c>
       <c r="G58" t="str">
-        <v>047</v>
+        <v>44047</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -1890,7 +1890,7 @@
         <v>44000</v>
       </c>
       <c r="G59" t="str">
-        <v>109</v>
+        <v>44109</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -1919,7 +1919,7 @@
         <v>44800</v>
       </c>
       <c r="G60" t="str">
-        <v>162</v>
+        <v>44162</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -1948,7 +1948,7 @@
         <v>44120</v>
       </c>
       <c r="G61" t="str">
-        <v>215</v>
+        <v>44215</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -1977,7 +1977,7 @@
         <v>44340</v>
       </c>
       <c r="G62" t="str">
-        <v>020</v>
+        <v>44020</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -2006,7 +2006,7 @@
         <v>44350</v>
       </c>
       <c r="G63" t="str">
-        <v>069</v>
+        <v>44069</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -2035,7 +2035,7 @@
         <v>49400</v>
       </c>
       <c r="G64" t="str">
-        <v>328</v>
+        <v>49328</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>49800</v>
       </c>
       <c r="G65" t="str">
-        <v>353</v>
+        <v>49353</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -2093,7 +2093,7 @@
         <v>85200</v>
       </c>
       <c r="G66" t="str">
-        <v>092</v>
+        <v>85092</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -2122,7 +2122,7 @@
         <v>85000</v>
       </c>
       <c r="G67" t="str">
-        <v>191</v>
+        <v>85191</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -2151,7 +2151,7 @@
         <v>72300</v>
       </c>
       <c r="G68" t="str">
-        <v>264</v>
+        <v>72264</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -2180,7 +2180,7 @@
         <v>44240</v>
       </c>
       <c r="G69" t="str">
-        <v>035</v>
+        <v>44035</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -2209,7 +2209,7 @@
         <v>44700</v>
       </c>
       <c r="G70" t="str">
-        <v>114</v>
+        <v>44114</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -2238,7 +2238,7 @@
         <v>44980</v>
       </c>
       <c r="G71" t="str">
-        <v>172</v>
+        <v>44172</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -2267,7 +2267,7 @@
         <v>44380</v>
       </c>
       <c r="G72" t="str">
-        <v>132</v>
+        <v>44132</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>44470</v>
       </c>
       <c r="G73" t="str">
-        <v>026</v>
+        <v>44026</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -2325,7 +2325,7 @@
         <v>85000</v>
       </c>
       <c r="G74" t="str">
-        <v>191</v>
+        <v>85191</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -2354,7 +2354,7 @@
         <v>44110</v>
       </c>
       <c r="G75" t="str">
-        <v>036</v>
+        <v>44036</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -2441,7 +2441,7 @@
         <v>53000</v>
       </c>
       <c r="G78" t="str">
-        <v>206</v>
+        <v>38206</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -2470,7 +2470,7 @@
         <v>72000</v>
       </c>
       <c r="G79" t="str">
-        <v>181</v>
+        <v>72181</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -2499,7 +2499,7 @@
         <v>44470</v>
       </c>
       <c r="G80" t="str">
-        <v>204</v>
+        <v>44204</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -2528,7 +2528,7 @@
         <v>44250</v>
       </c>
       <c r="G81" t="str">
-        <v>154</v>
+        <v>44154</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -2557,7 +2557,7 @@
         <v>37300</v>
       </c>
       <c r="G82" t="str">
-        <v>122</v>
+        <v>37122</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -2586,7 +2586,7 @@
         <v>18000</v>
       </c>
       <c r="G83" t="str">
-        <v>033</v>
+        <v>18033</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -2615,7 +2615,7 @@
         <v>28100</v>
       </c>
       <c r="G84" t="str">
-        <v>134</v>
+        <v>28134</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -2644,7 +2644,7 @@
         <v>41000</v>
       </c>
       <c r="G85" t="str">
-        <v>018</v>
+        <v>41018</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -2673,7 +2673,7 @@
         <v>45000</v>
       </c>
       <c r="G86" t="str">
-        <v>234</v>
+        <v>45234</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -2702,7 +2702,7 @@
         <v>37700</v>
       </c>
       <c r="G87" t="str">
-        <v>233</v>
+        <v>37233</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -2731,7 +2731,7 @@
         <v>36000</v>
       </c>
       <c r="G88" t="str">
-        <v>044</v>
+        <v>36044</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -2760,7 +2760,7 @@
         <v>37000</v>
       </c>
       <c r="G89" t="str">
-        <v>261</v>
+        <v>37261</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -2789,7 +2789,7 @@
         <v>45380</v>
       </c>
       <c r="G90" t="str">
-        <v>075</v>
+        <v>45075</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -2818,7 +2818,7 @@
         <v>45400</v>
       </c>
       <c r="G91" t="str">
-        <v>147</v>
+        <v>45147</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -2847,7 +2847,7 @@
         <v>45160</v>
       </c>
       <c r="G92" t="str">
-        <v>232</v>
+        <v>45232</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -2876,7 +2876,7 @@
         <v>28000</v>
       </c>
       <c r="G93" t="str">
-        <v>085</v>
+        <v>28085</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -2905,7 +2905,7 @@
         <v>37500</v>
       </c>
       <c r="G94" t="str">
-        <v>072</v>
+        <v>37072</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -2992,7 +2992,7 @@
         <v>97118</v>
       </c>
       <c r="G97" t="str">
-        <v>125</v>
+        <v>971125</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -3021,7 +3021,7 @@
         <v>97370</v>
       </c>
       <c r="G98" t="str">
-        <v>353</v>
+        <v>973353</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -3050,7 +3050,7 @@
         <v>97419</v>
       </c>
       <c r="G99" t="str">
-        <v>408</v>
+        <v>974408</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -3137,7 +3137,7 @@
         <v>97130</v>
       </c>
       <c r="G102" t="str">
-        <v>107</v>
+        <v>971107</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -3224,7 +3224,7 @@
         <v>38000</v>
       </c>
       <c r="G105" t="str">
-        <v>185</v>
+        <v>38185</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -3253,7 +3253,7 @@
         <v>38200</v>
       </c>
       <c r="G106" t="str">
-        <v>544</v>
+        <v>38544</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -3282,7 +3282,7 @@
         <v>63400</v>
       </c>
       <c r="G107" t="str">
-        <v>075</v>
+        <v>63075</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -3311,7 +3311,7 @@
         <v>63000</v>
       </c>
       <c r="G108" t="str">
-        <v>113</v>
+        <v>63113</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -3340,7 +3340,7 @@
         <v>38240</v>
       </c>
       <c r="G109" t="str">
-        <v>229</v>
+        <v>38229</v>
       </c>
       <c r="H109">
         <v>0</v>
@@ -3369,7 +3369,7 @@
         <v>42300</v>
       </c>
       <c r="G110" t="str">
-        <v>187</v>
+        <v>42187</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -3398,7 +3398,7 @@
         <v>26300</v>
       </c>
       <c r="G111" t="str">
-        <v>057</v>
+        <v>26057</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -3456,7 +3456,7 @@
         <v>69160</v>
       </c>
       <c r="G113" t="str">
-        <v>244</v>
+        <v>69244</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -3485,7 +3485,7 @@
         <v>74200</v>
       </c>
       <c r="G114" t="str">
-        <v>281</v>
+        <v>74281</v>
       </c>
       <c r="H114">
         <v>0</v>
@@ -3514,7 +3514,7 @@
         <v>1300</v>
       </c>
       <c r="G115" t="str">
-        <v>034</v>
+        <v>01034</v>
       </c>
       <c r="H115">
         <v>0</v>
@@ -3543,7 +3543,7 @@
         <v>1000</v>
       </c>
       <c r="G116" t="str">
-        <v>053</v>
+        <v>01053</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -3572,7 +3572,7 @@
         <v>1220</v>
       </c>
       <c r="G117" t="str">
-        <v>143</v>
+        <v>01143</v>
       </c>
       <c r="H117">
         <v>0</v>
@@ -3630,7 +3630,7 @@
         <v>38300</v>
       </c>
       <c r="G119" t="str">
-        <v>053</v>
+        <v>38053</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -3717,7 +3717,7 @@
         <v>69700</v>
       </c>
       <c r="G122" t="str">
-        <v>091</v>
+        <v>69091</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -3746,7 +3746,7 @@
         <v>69330</v>
       </c>
       <c r="G123" t="str">
-        <v>282</v>
+        <v>69282</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -3775,7 +3775,7 @@
         <v>69230</v>
       </c>
       <c r="G124" t="str">
-        <v>204</v>
+        <v>69204</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -3804,7 +3804,7 @@
         <v>26000</v>
       </c>
       <c r="G125" t="str">
-        <v>392</v>
+        <v>16392</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -3833,7 +3833,7 @@
         <v>42700</v>
       </c>
       <c r="G126" t="str">
-        <v>095</v>
+        <v>42095</v>
       </c>
       <c r="H126">
         <v>0</v>
@@ -3862,7 +3862,7 @@
         <v>26200</v>
       </c>
       <c r="G127" t="str">
-        <v>198</v>
+        <v>26198</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -3891,7 +3891,7 @@
         <v>74500</v>
       </c>
       <c r="G128" t="str">
-        <v>119</v>
+        <v>74119</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -3920,7 +3920,7 @@
         <v>26250</v>
       </c>
       <c r="G129" t="str">
-        <v>165</v>
+        <v>26165</v>
       </c>
       <c r="H129">
         <v>0</v>
@@ -3949,7 +3949,7 @@
         <v>69100</v>
       </c>
       <c r="G130" t="str">
-        <v>266</v>
+        <v>69266</v>
       </c>
       <c r="H130">
         <v>0</v>
@@ -4036,7 +4036,7 @@
         <v>63500</v>
       </c>
       <c r="G133" t="str">
-        <v>178</v>
+        <v>63178</v>
       </c>
       <c r="H133">
         <v>0</v>
@@ -4065,7 +4065,7 @@
         <v>38600</v>
       </c>
       <c r="G134" t="str">
-        <v>150</v>
+        <v>10150</v>
       </c>
       <c r="H134">
         <v>0</v>
@@ -4094,7 +4094,7 @@
         <v>73300</v>
       </c>
       <c r="G135" t="str">
-        <v>248</v>
+        <v>73248</v>
       </c>
       <c r="H135">
         <v>0</v>
@@ -4123,7 +4123,7 @@
         <v>63200</v>
       </c>
       <c r="G136" t="str">
-        <v>300</v>
+        <v>63300</v>
       </c>
       <c r="H136">
         <v>0</v>
@@ -4152,7 +4152,7 @@
         <v>74000</v>
       </c>
       <c r="G137" t="str">
-        <v>010</v>
+        <v>74010</v>
       </c>
       <c r="H137">
         <v>0</v>
@@ -4181,7 +4181,7 @@
         <v>1210</v>
       </c>
       <c r="G138" t="str">
-        <v>160</v>
+        <v>01160</v>
       </c>
       <c r="H138">
         <v>0</v>
@@ -4210,7 +4210,7 @@
         <v>7300</v>
       </c>
       <c r="G139" t="str">
-        <v>324</v>
+        <v>07324</v>
       </c>
       <c r="H139">
         <v>0</v>
@@ -4239,7 +4239,7 @@
         <v>15000</v>
       </c>
       <c r="G140" t="str">
-        <v>014</v>
+        <v>15014</v>
       </c>
       <c r="H140">
         <v>0</v>
@@ -4297,7 +4297,7 @@
         <v>42230</v>
       </c>
       <c r="G142" t="str">
-        <v>189</v>
+        <v>42189</v>
       </c>
       <c r="H142">
         <v>0</v>
@@ -4326,7 +4326,7 @@
         <v>73100</v>
       </c>
       <c r="G143" t="str">
-        <v>008</v>
+        <v>73008</v>
       </c>
       <c r="H143">
         <v>0</v>
@@ -4355,7 +4355,7 @@
         <v>69700</v>
       </c>
       <c r="G144" t="str">
-        <v>091</v>
+        <v>69091</v>
       </c>
       <c r="H144">
         <v>0</v>
@@ -4384,7 +4384,7 @@
         <v>63170</v>
       </c>
       <c r="G145" t="str">
-        <v>014</v>
+        <v>63014</v>
       </c>
       <c r="H145">
         <v>0</v>
@@ -4413,7 +4413,7 @@
         <v>1170</v>
       </c>
       <c r="G146" t="str">
-        <v>173</v>
+        <v>01173</v>
       </c>
       <c r="H146">
         <v>0</v>
@@ -4442,7 +4442,7 @@
         <v>69150</v>
       </c>
       <c r="G147" t="str">
-        <v>275</v>
+        <v>69275</v>
       </c>
       <c r="H147">
         <v>0</v>
@@ -4471,7 +4471,7 @@
         <v>69780</v>
       </c>
       <c r="G148" t="str">
-        <v>283</v>
+        <v>69283</v>
       </c>
       <c r="H148">
         <v>0</v>
@@ -4500,7 +4500,7 @@
         <v>3100</v>
       </c>
       <c r="G149" t="str">
-        <v>185</v>
+        <v>03185</v>
       </c>
       <c r="H149">
         <v>0</v>
@@ -4529,7 +4529,7 @@
         <v>69600</v>
       </c>
       <c r="G150" t="str">
-        <v>149</v>
+        <v>69149</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -4558,7 +4558,7 @@
         <v>69330</v>
       </c>
       <c r="G151" t="str">
-        <v>282</v>
+        <v>69282</v>
       </c>
       <c r="H151">
         <v>0</v>
@@ -4645,7 +4645,7 @@
         <v>69500</v>
       </c>
       <c r="G154" t="str">
-        <v>029</v>
+        <v>69029</v>
       </c>
       <c r="H154">
         <v>0</v>
@@ -4674,7 +4674,7 @@
         <v>69200</v>
       </c>
       <c r="G155" t="str">
-        <v>259</v>
+        <v>69259</v>
       </c>
       <c r="H155">
         <v>0</v>
@@ -4703,7 +4703,7 @@
         <v>69340</v>
       </c>
       <c r="G156" t="str">
-        <v>284</v>
+        <v>21284</v>
       </c>
       <c r="H156">
         <v>0</v>
@@ -4732,7 +4732,7 @@
         <v>69110</v>
       </c>
       <c r="G157" t="str">
-        <v>202</v>
+        <v>69202</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -4761,7 +4761,7 @@
         <v>1700</v>
       </c>
       <c r="G158" t="str">
-        <v>249</v>
+        <v>01249</v>
       </c>
       <c r="H158">
         <v>0</v>
@@ -4790,7 +4790,7 @@
         <v>69230</v>
       </c>
       <c r="G159" t="str">
-        <v>204</v>
+        <v>69204</v>
       </c>
       <c r="H159">
         <v>0</v>
@@ -5080,7 +5080,7 @@
         <v>25000</v>
       </c>
       <c r="G169" t="str">
-        <v>056</v>
+        <v>25056</v>
       </c>
       <c r="H169">
         <v>0</v>
@@ -5109,7 +5109,7 @@
         <v>39000</v>
       </c>
       <c r="G170" t="str">
-        <v>300</v>
+        <v>39300</v>
       </c>
       <c r="H170">
         <v>0</v>
@@ -5138,7 +5138,7 @@
         <v>89110</v>
       </c>
       <c r="G171" t="str">
-        <v>360</v>
+        <v>89360</v>
       </c>
       <c r="H171">
         <v>0</v>
@@ -5167,7 +5167,7 @@
         <v>70000</v>
       </c>
       <c r="G172" t="str">
-        <v>550</v>
+        <v>70550</v>
       </c>
       <c r="H172">
         <v>0</v>
@@ -5196,7 +5196,7 @@
         <v>21200</v>
       </c>
       <c r="G173" t="str">
-        <v>054</v>
+        <v>21054</v>
       </c>
       <c r="H173">
         <v>0</v>
@@ -5254,7 +5254,7 @@
         <v>25300</v>
       </c>
       <c r="G175" t="str">
-        <v>462</v>
+        <v>25462</v>
       </c>
       <c r="H175">
         <v>0</v>
@@ -5283,7 +5283,7 @@
         <v>58000</v>
       </c>
       <c r="G176" t="str">
-        <v>194</v>
+        <v>58194</v>
       </c>
       <c r="H176">
         <v>0</v>
@@ -5312,7 +5312,7 @@
         <v>89100</v>
       </c>
       <c r="G177" t="str">
-        <v>387</v>
+        <v>89387</v>
       </c>
       <c r="H177">
         <v>0</v>
@@ -5341,7 +5341,7 @@
         <v>89000</v>
       </c>
       <c r="G178" t="str">
-        <v>024</v>
+        <v>89024</v>
       </c>
       <c r="H178">
         <v>0</v>
@@ -5370,7 +5370,7 @@
         <v>21000</v>
       </c>
       <c r="G179" t="str">
-        <v>231</v>
+        <v>21231</v>
       </c>
       <c r="H179">
         <v>0</v>
@@ -5428,7 +5428,7 @@
         <v>25200</v>
       </c>
       <c r="G181" t="str">
-        <v>388</v>
+        <v>25388</v>
       </c>
       <c r="H181">
         <v>0</v>
@@ -5457,7 +5457,7 @@
         <v>90000</v>
       </c>
       <c r="G182" t="str">
-        <v>010</v>
+        <v>90010</v>
       </c>
       <c r="H182">
         <v>0</v>
@@ -5486,7 +5486,7 @@
         <v>39100</v>
       </c>
       <c r="G183" t="str">
-        <v>198</v>
+        <v>39198</v>
       </c>
       <c r="H183">
         <v>0</v>
@@ -5515,7 +5515,7 @@
         <v>21800</v>
       </c>
       <c r="G184" t="str">
-        <v>171</v>
+        <v>21171</v>
       </c>
       <c r="H184">
         <v>0</v>
@@ -5544,7 +5544,7 @@
         <v>71400</v>
       </c>
       <c r="G185" t="str">
-        <v>014</v>
+        <v>71014</v>
       </c>
       <c r="H185">
         <v>0</v>
@@ -5573,7 +5573,7 @@
         <v>57190</v>
       </c>
       <c r="G186" t="str">
-        <v>221</v>
+        <v>57221</v>
       </c>
       <c r="H186">
         <v>0</v>
@@ -5602,7 +5602,7 @@
         <v>10000</v>
       </c>
       <c r="G187" t="str">
-        <v>387</v>
+        <v>10387</v>
       </c>
       <c r="H187">
         <v>0</v>
@@ -5631,7 +5631,7 @@
         <v>57600</v>
       </c>
       <c r="G188" t="str">
-        <v>227</v>
+        <v>57227</v>
       </c>
       <c r="H188">
         <v>0</v>
@@ -5660,7 +5660,7 @@
         <v>51100</v>
       </c>
       <c r="G189" t="str">
-        <v>454</v>
+        <v>51454</v>
       </c>
       <c r="H189">
         <v>0</v>
@@ -5689,7 +5689,7 @@
         <v>52100</v>
       </c>
       <c r="G190" t="str">
-        <v>448</v>
+        <v>52448</v>
       </c>
       <c r="H190">
         <v>0</v>
@@ -5718,7 +5718,7 @@
         <v>67300</v>
       </c>
       <c r="G191" t="str">
-        <v>447</v>
+        <v>67447</v>
       </c>
       <c r="H191">
         <v>0</v>
@@ -5747,7 +5747,7 @@
         <v>68700</v>
       </c>
       <c r="G192" t="str">
-        <v>147</v>
+        <v>14147</v>
       </c>
       <c r="H192">
         <v>0</v>
@@ -5776,7 +5776,7 @@
         <v>57155</v>
       </c>
       <c r="G193" t="str">
-        <v>447</v>
+        <v>57447</v>
       </c>
       <c r="H193">
         <v>0</v>
@@ -5834,7 +5834,7 @@
         <v>68000</v>
       </c>
       <c r="G195" t="str">
-        <v>066</v>
+        <v>68066</v>
       </c>
       <c r="H195">
         <v>0</v>
@@ -5863,7 +5863,7 @@
         <v>57000</v>
       </c>
       <c r="G196" t="str">
-        <v>463</v>
+        <v>57463</v>
       </c>
       <c r="H196">
         <v>0</v>
@@ -5892,7 +5892,7 @@
         <v>68100</v>
       </c>
       <c r="G197" t="str">
-        <v>224</v>
+        <v>68224</v>
       </c>
       <c r="H197">
         <v>0</v>
@@ -5950,7 +5950,7 @@
         <v>8200</v>
       </c>
       <c r="G199" t="str">
-        <v>409</v>
+        <v>08409</v>
       </c>
       <c r="H199">
         <v>0</v>
@@ -5979,7 +5979,7 @@
         <v>67000</v>
       </c>
       <c r="G200" t="str">
-        <v>482</v>
+        <v>67482</v>
       </c>
       <c r="H200">
         <v>0</v>
@@ -6008,7 +6008,7 @@
         <v>10200</v>
       </c>
       <c r="G201" t="str">
-        <v>033</v>
+        <v>10033</v>
       </c>
       <c r="H201">
         <v>0</v>
@@ -6037,7 +6037,7 @@
         <v>54000</v>
       </c>
       <c r="G202" t="str">
-        <v>395</v>
+        <v>54395</v>
       </c>
       <c r="H202">
         <v>0</v>
@@ -6066,7 +6066,7 @@
         <v>54600</v>
       </c>
       <c r="G203" t="str">
-        <v>578</v>
+        <v>54578</v>
       </c>
       <c r="H203">
         <v>0</v>
@@ -6095,7 +6095,7 @@
         <v>54500</v>
       </c>
       <c r="G204" t="str">
-        <v>547</v>
+        <v>54547</v>
       </c>
       <c r="H204">
         <v>0</v>
@@ -6124,7 +6124,7 @@
         <v>51300</v>
       </c>
       <c r="G205" t="str">
-        <v>649</v>
+        <v>51649</v>
       </c>
       <c r="H205">
         <v>0</v>
@@ -6153,7 +6153,7 @@
         <v>55000</v>
       </c>
       <c r="G206" t="str">
-        <v>029</v>
+        <v>55029</v>
       </c>
       <c r="H206">
         <v>0</v>
@@ -6182,7 +6182,7 @@
         <v>54400</v>
       </c>
       <c r="G207" t="str">
-        <v>323</v>
+        <v>54323</v>
       </c>
       <c r="H207">
         <v>0</v>
@@ -6211,7 +6211,7 @@
         <v>57200</v>
       </c>
       <c r="G208" t="str">
-        <v>631</v>
+        <v>57631</v>
       </c>
       <c r="H208">
         <v>0</v>
@@ -6240,7 +6240,7 @@
         <v>54700</v>
       </c>
       <c r="G209" t="str">
-        <v>431</v>
+        <v>54431</v>
       </c>
       <c r="H209">
         <v>0</v>
@@ -6269,7 +6269,7 @@
         <v>67240</v>
       </c>
       <c r="G210" t="str">
-        <v>046</v>
+        <v>67046</v>
       </c>
       <c r="H210">
         <v>0</v>
@@ -6298,7 +6298,7 @@
         <v>54320</v>
       </c>
       <c r="G211" t="str">
-        <v>357</v>
+        <v>54357</v>
       </c>
       <c r="H211">
         <v>0</v>
@@ -6327,7 +6327,7 @@
         <v>93210</v>
       </c>
       <c r="G212" t="str">
-        <v>339</v>
+        <v>11339</v>
       </c>
     </row>
     <row r="213">
@@ -6350,7 +6350,7 @@
         <v>93400</v>
       </c>
       <c r="G213" t="str">
-        <v>226</v>
+        <v>41226</v>
       </c>
     </row>
     <row r="214">
@@ -6373,7 +6373,7 @@
         <v>77330</v>
       </c>
       <c r="G214" t="str">
-        <v>350</v>
+        <v>77350</v>
       </c>
     </row>
     <row r="215">
@@ -6396,7 +6396,7 @@
         <v>78418</v>
       </c>
       <c r="G215" t="str">
-        <v>418</v>
+        <v>78418</v>
       </c>
     </row>
     <row r="216">
@@ -6442,7 +6442,7 @@
         <v>92300</v>
       </c>
       <c r="G217" t="str">
-        <v>044</v>
+        <v>92044</v>
       </c>
     </row>
     <row r="218">
@@ -6465,7 +6465,7 @@
         <v>92800</v>
       </c>
       <c r="G218" t="str">
-        <v>062</v>
+        <v>92062</v>
       </c>
     </row>
     <row r="219">
@@ -6488,7 +6488,7 @@
         <v>95370</v>
       </c>
       <c r="G219" t="str">
-        <v>424</v>
+        <v>95424</v>
       </c>
       <c r="I219" t="str">
         <v>https://actu.fr/ile-de-france/montigny-les-cormeilles_95424/val-doise-municipales-2020-jean-noel-carpentier-brigue-troisieme-mandat_29870776.html</v>
@@ -6514,7 +6514,7 @@
         <v>94120</v>
       </c>
       <c r="G220" t="str">
-        <v>033</v>
+        <v>94033</v>
       </c>
     </row>
     <row r="221">
@@ -6537,7 +6537,7 @@
         <v>78800</v>
       </c>
       <c r="G221" t="str">
-        <v>311</v>
+        <v>78311</v>
       </c>
     </row>
     <row r="222">
@@ -6560,7 +6560,7 @@
         <v>95880</v>
       </c>
       <c r="G222" t="str">
-        <v>210</v>
+        <v>95210</v>
       </c>
     </row>
     <row r="223">
@@ -6606,7 +6606,7 @@
         <v>93500</v>
       </c>
       <c r="G224" t="str">
-        <v>055</v>
+        <v>93055</v>
       </c>
     </row>
     <row r="225">
@@ -6629,7 +6629,7 @@
         <v>92160</v>
       </c>
       <c r="G225" t="str">
-        <v>002</v>
+        <v>92002</v>
       </c>
     </row>
     <row r="226">
@@ -6652,7 +6652,7 @@
         <v>92330</v>
       </c>
       <c r="G226" t="str">
-        <v>071</v>
+        <v>92071</v>
       </c>
     </row>
     <row r="227">
@@ -6675,7 +6675,7 @@
         <v>93330</v>
       </c>
       <c r="G227" t="str">
-        <v>050</v>
+        <v>93050</v>
       </c>
     </row>
     <row r="228">
@@ -6698,7 +6698,7 @@
         <v>95600</v>
       </c>
       <c r="G228" t="str">
-        <v>203</v>
+        <v>95203</v>
       </c>
     </row>
     <row r="229">
@@ -6721,7 +6721,7 @@
         <v>77170</v>
       </c>
       <c r="G229" t="str">
-        <v>053</v>
+        <v>77053</v>
       </c>
     </row>
     <row r="230">
@@ -6744,7 +6744,7 @@
         <v>78520</v>
       </c>
       <c r="G230" t="str">
-        <v>335</v>
+        <v>78335</v>
       </c>
     </row>
     <row r="231">
@@ -6767,7 +6767,7 @@
         <v>94160</v>
       </c>
       <c r="G231" t="str">
-        <v>067</v>
+        <v>94067</v>
       </c>
     </row>
     <row r="232">
@@ -6790,7 +6790,7 @@
         <v>94300</v>
       </c>
       <c r="G232" t="str">
-        <v>080</v>
+        <v>94080</v>
       </c>
     </row>
     <row r="233">
@@ -6813,7 +6813,7 @@
         <v>93600</v>
       </c>
       <c r="G233" t="str">
-        <v>005</v>
+        <v>93005</v>
       </c>
     </row>
     <row r="234">
@@ -6836,7 +6836,7 @@
         <v>91200</v>
       </c>
       <c r="G234" t="str">
-        <v>027</v>
+        <v>91027</v>
       </c>
     </row>
     <row r="235">
@@ -6859,7 +6859,7 @@
         <v>94360</v>
       </c>
       <c r="G235" t="str">
-        <v>015</v>
+        <v>94015</v>
       </c>
     </row>
     <row r="236">
@@ -6905,7 +6905,7 @@
         <v>91370</v>
       </c>
       <c r="G237" t="str">
-        <v>645</v>
+        <v>91645</v>
       </c>
       <c r="H237" t="str">
         <v>https://www.reussirensembleverrieres.fr/notre-candidat-vincent-hulin/</v>
@@ -6931,7 +6931,7 @@
         <v>91600</v>
       </c>
       <c r="G238" t="str">
-        <v>589</v>
+        <v>91589</v>
       </c>
     </row>
     <row r="239">
@@ -6954,7 +6954,7 @@
         <v>94200</v>
       </c>
       <c r="G239" t="str">
-        <v>041</v>
+        <v>94041</v>
       </c>
     </row>
     <row r="240">
@@ -6977,7 +6977,7 @@
         <v>92220</v>
       </c>
       <c r="G240" t="str">
-        <v>043</v>
+        <v>02043</v>
       </c>
     </row>
     <row r="241">
@@ -7000,7 +7000,7 @@
         <v>93390</v>
       </c>
       <c r="G241" t="str">
-        <v>014</v>
+        <v>93014</v>
       </c>
     </row>
     <row r="242">
@@ -7020,7 +7020,7 @@
         <v>94550</v>
       </c>
       <c r="G242" t="str">
-        <v>021</v>
+        <v>94021</v>
       </c>
     </row>
     <row r="243">
@@ -7043,7 +7043,7 @@
         <v>77420</v>
       </c>
       <c r="G243" t="str">
-        <v>083</v>
+        <v>77083</v>
       </c>
     </row>
     <row r="244">
@@ -7089,7 +7089,7 @@
         <v>95350</v>
       </c>
       <c r="G245" t="str">
-        <v>539</v>
+        <v>95539</v>
       </c>
     </row>
     <row r="246">
@@ -7112,7 +7112,7 @@
         <v>94230</v>
       </c>
       <c r="G246" t="str">
-        <v>016</v>
+        <v>94016</v>
       </c>
     </row>
     <row r="247">
@@ -7135,7 +7135,7 @@
         <v>95130</v>
       </c>
       <c r="G247" t="str">
-        <v>209</v>
+        <v>54209</v>
       </c>
     </row>
     <row r="248">
@@ -7181,7 +7181,7 @@
         <v>77360</v>
       </c>
       <c r="G249" t="str">
-        <v>479</v>
+        <v>77479</v>
       </c>
     </row>
     <row r="250">
@@ -7204,7 +7204,7 @@
         <v>94510</v>
       </c>
       <c r="G250" t="str">
-        <v>060</v>
+        <v>94060</v>
       </c>
     </row>
     <row r="251">
@@ -7227,7 +7227,7 @@
         <v>91190</v>
       </c>
       <c r="G251" t="str">
-        <v>272</v>
+        <v>91272</v>
       </c>
     </row>
     <row r="252">
@@ -7250,7 +7250,7 @@
         <v>91270</v>
       </c>
       <c r="G252" t="str">
-        <v>657</v>
+        <v>91657</v>
       </c>
     </row>
     <row r="253">
@@ -7273,7 +7273,7 @@
         <v>95160</v>
       </c>
       <c r="G253" t="str">
-        <v>428</v>
+        <v>95428</v>
       </c>
     </row>
     <row r="254">
@@ -7296,7 +7296,7 @@
         <v>91100</v>
       </c>
       <c r="G254" t="str">
-        <v>174</v>
+        <v>91174</v>
       </c>
     </row>
     <row r="255">
@@ -7319,7 +7319,7 @@
         <v>92310</v>
       </c>
       <c r="G255" t="str">
-        <v>072</v>
+        <v>92072</v>
       </c>
     </row>
     <row r="256">
@@ -7342,7 +7342,7 @@
         <v>77380</v>
       </c>
       <c r="G256" t="str">
-        <v>122</v>
+        <v>77122</v>
       </c>
     </row>
     <row r="257">
@@ -7365,7 +7365,7 @@
         <v>93420</v>
       </c>
       <c r="G257" t="str">
-        <v>434</v>
+        <v>11434</v>
       </c>
     </row>
     <row r="258">
@@ -7388,7 +7388,7 @@
         <v>78120</v>
       </c>
       <c r="G258" t="str">
-        <v>517</v>
+        <v>78517</v>
       </c>
     </row>
     <row r="259">
@@ -7411,7 +7411,7 @@
         <v>94500</v>
       </c>
       <c r="G259" t="str">
-        <v>017</v>
+        <v>94017</v>
       </c>
     </row>
     <row r="260">
@@ -7434,7 +7434,7 @@
         <v>92400</v>
       </c>
       <c r="G260" t="str">
-        <v>026</v>
+        <v>92026</v>
       </c>
     </row>
     <row r="261">
@@ -7457,7 +7457,7 @@
         <v>94320</v>
       </c>
       <c r="G261" t="str">
-        <v>073</v>
+        <v>94073</v>
       </c>
     </row>
     <row r="262">
@@ -7480,7 +7480,7 @@
         <v>94260</v>
       </c>
       <c r="G262" t="str">
-        <v>287</v>
+        <v>21287</v>
       </c>
     </row>
     <row r="263">
@@ -7503,7 +7503,7 @@
         <v>95540</v>
       </c>
       <c r="G263" t="str">
-        <v>394</v>
+        <v>95394</v>
       </c>
     </row>
     <row r="264">
@@ -7569,7 +7569,7 @@
         <v>78510</v>
       </c>
       <c r="G266" t="str">
-        <v>624</v>
+        <v>78624</v>
       </c>
     </row>
     <row r="267">
@@ -7589,7 +7589,7 @@
         <v>92600</v>
       </c>
       <c r="G267" t="str">
-        <v>004</v>
+        <v>92004</v>
       </c>
     </row>
     <row r="268">
@@ -7609,7 +7609,7 @@
         <v>92700</v>
       </c>
       <c r="G268" t="str">
-        <v>025</v>
+        <v>92025</v>
       </c>
     </row>
     <row r="269">
@@ -7649,7 +7649,7 @@
         <v>78400</v>
       </c>
       <c r="G270" t="str">
-        <v>146</v>
+        <v>78146</v>
       </c>
     </row>
     <row r="271">
@@ -7669,7 +7669,7 @@
         <v>78160</v>
       </c>
       <c r="G271" t="str">
-        <v>372</v>
+        <v>78372</v>
       </c>
     </row>
     <row r="272">
@@ -7689,7 +7689,7 @@
         <v>78100</v>
       </c>
       <c r="G272" t="str">
-        <v>551</v>
+        <v>78551</v>
       </c>
     </row>
     <row r="273">
@@ -7709,7 +7709,7 @@
         <v>78540</v>
       </c>
       <c r="G273" t="str">
-        <v>404</v>
+        <v>28404</v>
       </c>
     </row>
     <row r="274">
@@ -7729,7 +7729,7 @@
         <v>92340</v>
       </c>
       <c r="G274" t="str">
-        <v>014</v>
+        <v>92014</v>
       </c>
     </row>
     <row r="275">
@@ -7749,7 +7749,7 @@
         <v>92240</v>
       </c>
       <c r="G275" t="str">
-        <v>046</v>
+        <v>92046</v>
       </c>
     </row>
     <row r="276">
@@ -7769,7 +7769,7 @@
         <v>94470</v>
       </c>
       <c r="G276" t="str">
-        <v>004</v>
+        <v>94004</v>
       </c>
     </row>
     <row r="277">
@@ -7789,7 +7789,7 @@
         <v>94700</v>
       </c>
       <c r="G277" t="str">
-        <v>046</v>
+        <v>94046</v>
       </c>
     </row>
     <row r="278">
@@ -7809,7 +7809,7 @@
         <v>94170</v>
       </c>
       <c r="G278" t="str">
-        <v>058</v>
+        <v>94058</v>
       </c>
     </row>
     <row r="279">
@@ -7829,7 +7829,7 @@
         <v>95360</v>
       </c>
       <c r="G279" t="str">
-        <v>427</v>
+        <v>95427</v>
       </c>
     </row>
     <row r="280">
@@ -7849,7 +7849,7 @@
         <v>92170</v>
       </c>
       <c r="G280" t="str">
-        <v>075</v>
+        <v>92075</v>
       </c>
     </row>
     <row r="281">
@@ -7869,7 +7869,7 @@
         <v>77176</v>
       </c>
       <c r="G281" t="str">
-        <v>445</v>
+        <v>77445</v>
       </c>
     </row>
     <row r="282">
@@ -7889,7 +7889,7 @@
         <v>78280</v>
       </c>
       <c r="G282" t="str">
-        <v>297</v>
+        <v>78297</v>
       </c>
     </row>
     <row r="283">
@@ -7909,7 +7909,7 @@
         <v>93340</v>
       </c>
       <c r="G283" t="str">
-        <v>062</v>
+        <v>93062</v>
       </c>
     </row>
     <row r="284">
@@ -7929,7 +7929,7 @@
         <v>78150</v>
       </c>
       <c r="G284" t="str">
-        <v>158</v>
+        <v>78158</v>
       </c>
     </row>
     <row r="285">
@@ -7969,7 +7969,7 @@
         <v>92120</v>
       </c>
       <c r="G286" t="str">
-        <v>049</v>
+        <v>92049</v>
       </c>
     </row>
     <row r="287">
@@ -7989,7 +7989,7 @@
         <v>93250</v>
       </c>
       <c r="G287" t="str">
-        <v>077</v>
+        <v>93077</v>
       </c>
     </row>
     <row r="288">
@@ -8009,7 +8009,7 @@
         <v>92500</v>
       </c>
       <c r="G288" t="str">
-        <v>063</v>
+        <v>92063</v>
       </c>
     </row>
     <row r="289">
@@ -8029,7 +8029,7 @@
         <v>78480</v>
       </c>
       <c r="G289" t="str">
-        <v>642</v>
+        <v>78642</v>
       </c>
     </row>
     <row r="290">
@@ -8049,7 +8049,7 @@
         <v>78955</v>
       </c>
       <c r="G290" t="str">
-        <v>123</v>
+        <v>78123</v>
       </c>
     </row>
     <row r="291">
@@ -8069,7 +8069,7 @@
         <v>92270</v>
       </c>
       <c r="G291" t="str">
-        <v>009</v>
+        <v>92009</v>
       </c>
     </row>
     <row r="292">
@@ -8089,7 +8089,7 @@
         <v>92210</v>
       </c>
       <c r="G292" t="str">
-        <v>064</v>
+        <v>92064</v>
       </c>
     </row>
     <row r="293">
@@ -8109,7 +8109,7 @@
         <v>92000</v>
       </c>
       <c r="G293" t="str">
-        <v>050</v>
+        <v>92050</v>
       </c>
     </row>
     <row r="294">
@@ -8129,7 +8129,7 @@
         <v>95320</v>
       </c>
       <c r="G294" t="str">
-        <v>563</v>
+        <v>95563</v>
       </c>
     </row>
     <row r="295">
@@ -8169,7 +8169,7 @@
         <v>78711</v>
       </c>
       <c r="G296" t="str">
-        <v>362</v>
+        <v>78362</v>
       </c>
     </row>
     <row r="297">
@@ -8189,7 +8189,7 @@
         <v>78600</v>
       </c>
       <c r="G297" t="str">
-        <v>358</v>
+        <v>78358</v>
       </c>
     </row>
     <row r="298">
@@ -8209,7 +8209,7 @@
         <v>92390</v>
       </c>
       <c r="G298" t="str">
-        <v>078</v>
+        <v>92078</v>
       </c>
     </row>
     <row r="299">
@@ -8229,7 +8229,7 @@
         <v>93260</v>
       </c>
       <c r="G299" t="str">
-        <v>045</v>
+        <v>93045</v>
       </c>
     </row>
     <row r="300">
@@ -8249,7 +8249,7 @@
         <v>77144</v>
       </c>
       <c r="G300" t="str">
-        <v>307</v>
+        <v>77307</v>
       </c>
     </row>
     <row r="301">
@@ -8266,7 +8266,7 @@
         <v>Pontault-Combault</v>
       </c>
       <c r="G301" t="str">
-        <v>373</v>
+        <v>77373</v>
       </c>
     </row>
     <row r="302">
@@ -8283,7 +8283,7 @@
         <v>Saint-Pierre-du-Perray</v>
       </c>
       <c r="G302" t="str">
-        <v>573</v>
+        <v>91573</v>
       </c>
     </row>
     <row r="303">
@@ -8334,7 +8334,7 @@
         <v>Argenteuil</v>
       </c>
       <c r="G305" t="str">
-        <v>018</v>
+        <v>95018</v>
       </c>
     </row>
     <row r="306">
@@ -8351,7 +8351,7 @@
         <v>Fontainebleau</v>
       </c>
       <c r="G306" t="str">
-        <v>186</v>
+        <v>77186</v>
       </c>
     </row>
     <row r="307">
@@ -8368,7 +8368,7 @@
         <v>Montreuil</v>
       </c>
       <c r="G307" t="str">
-        <v>267</v>
+        <v>28267</v>
       </c>
     </row>
     <row r="308">
@@ -8385,7 +8385,7 @@
         <v>Brétigny-sur-Orge</v>
       </c>
       <c r="G308" t="str">
-        <v>103</v>
+        <v>91103</v>
       </c>
     </row>
     <row r="309">
@@ -8419,7 +8419,7 @@
         <v>Igny</v>
       </c>
       <c r="G310" t="str">
-        <v>289</v>
+        <v>70289</v>
       </c>
     </row>
     <row r="311">
@@ -8436,7 +8436,7 @@
         <v>Massy</v>
       </c>
       <c r="G311" t="str">
-        <v>415</v>
+        <v>76415</v>
       </c>
     </row>
     <row r="312">
@@ -8453,7 +8453,7 @@
         <v>Mennecy</v>
       </c>
       <c r="G312" t="str">
-        <v>386</v>
+        <v>91386</v>
       </c>
     </row>
     <row r="313">
@@ -8470,7 +8470,7 @@
         <v>Ris-Orangis</v>
       </c>
       <c r="G313" t="str">
-        <v>521</v>
+        <v>91521</v>
       </c>
     </row>
     <row r="314">
@@ -8504,7 +8504,7 @@
         <v>Les Ulis</v>
       </c>
       <c r="G315" t="str">
-        <v>692</v>
+        <v>91692</v>
       </c>
     </row>
     <row r="316">
@@ -8521,7 +8521,7 @@
         <v>Palaiseau</v>
       </c>
       <c r="G316" t="str">
-        <v>477</v>
+        <v>91477</v>
       </c>
     </row>
     <row r="317">
@@ -8538,7 +8538,7 @@
         <v>Moissy-Cramayel</v>
       </c>
       <c r="G317" t="str">
-        <v>296</v>
+        <v>77296</v>
       </c>
     </row>
     <row r="318">
@@ -8555,7 +8555,7 @@
         <v>Clamart</v>
       </c>
       <c r="G318" t="str">
-        <v>023</v>
+        <v>92023</v>
       </c>
     </row>
     <row r="319">
@@ -8572,7 +8572,7 @@
         <v>La Garenne-Colombes</v>
       </c>
       <c r="G319" t="str">
-        <v>035</v>
+        <v>92035</v>
       </c>
     </row>
     <row r="320">
@@ -8589,7 +8589,7 @@
         <v>Neuilly-sur-Seine</v>
       </c>
       <c r="G320" t="str">
-        <v>051</v>
+        <v>92051</v>
       </c>
     </row>
     <row r="321">
@@ -8606,7 +8606,7 @@
         <v>Bagnolet</v>
       </c>
       <c r="G321" t="str">
-        <v>006</v>
+        <v>93006</v>
       </c>
     </row>
     <row r="322">
@@ -8623,7 +8623,7 @@
         <v>Gentilly</v>
       </c>
       <c r="G322" t="str">
-        <v>037</v>
+        <v>94037</v>
       </c>
     </row>
     <row r="323">
@@ -8657,7 +8657,7 @@
         <v>Saint-Maurice</v>
       </c>
       <c r="G324" t="str">
-        <v>453</v>
+        <v>52453</v>
       </c>
     </row>
     <row r="325">
@@ -8674,7 +8674,7 @@
         <v>Sucy-en-Brie</v>
       </c>
       <c r="G325" t="str">
-        <v>071</v>
+        <v>94071</v>
       </c>
     </row>
     <row r="326">
@@ -8691,7 +8691,7 @@
         <v>Lagny-sur-Marne</v>
       </c>
       <c r="G326" t="str">
-        <v>243</v>
+        <v>77243</v>
       </c>
     </row>
     <row r="327">
@@ -8708,7 +8708,7 @@
         <v>Chelles</v>
       </c>
       <c r="G327" t="str">
-        <v>145</v>
+        <v>60145</v>
       </c>
     </row>
     <row r="328">
@@ -8725,7 +8725,7 @@
         <v>Pontault-Combault</v>
       </c>
       <c r="G328" t="str">
-        <v>373</v>
+        <v>77373</v>
       </c>
     </row>
     <row r="329">
@@ -8742,7 +8742,7 @@
         <v>Roissy-en-Brie</v>
       </c>
       <c r="G329" t="str">
-        <v>390</v>
+        <v>77390</v>
       </c>
     </row>
     <row r="330">
@@ -8759,7 +8759,7 @@
         <v>Romainville</v>
       </c>
       <c r="G330" t="str">
-        <v>063</v>
+        <v>93063</v>
       </c>
     </row>
     <row r="331">
@@ -8776,7 +8776,7 @@
         <v>Joinville-le-Pont</v>
       </c>
       <c r="G331" t="str">
-        <v>042</v>
+        <v>94042</v>
       </c>
     </row>
     <row r="332">
@@ -8793,7 +8793,7 @@
         <v>Saint-Maur-des-Fossés</v>
       </c>
       <c r="G332" t="str">
-        <v>068</v>
+        <v>94068</v>
       </c>
     </row>
     <row r="333">
@@ -8810,7 +8810,7 @@
         <v>Gonesse</v>
       </c>
       <c r="G333" t="str">
-        <v>277</v>
+        <v>95277</v>
       </c>
     </row>
     <row r="334">
@@ -8827,7 +8827,7 @@
         <v>Bezons</v>
       </c>
       <c r="G334" t="str">
-        <v>063</v>
+        <v>95063</v>
       </c>
     </row>
     <row r="335">
@@ -8844,7 +8844,7 @@
         <v>Melun</v>
       </c>
       <c r="G335" t="str">
-        <v>288</v>
+        <v>77288</v>
       </c>
     </row>
     <row r="336">
@@ -8861,7 +8861,7 @@
         <v>Soisy-sous-Montmorency</v>
       </c>
       <c r="G336" t="str">
-        <v>598</v>
+        <v>95598</v>
       </c>
     </row>
     <row r="337">
@@ -8895,7 +8895,7 @@
         <v>Longjumeau</v>
       </c>
       <c r="G338" t="str">
-        <v>345</v>
+        <v>91345</v>
       </c>
     </row>
     <row r="339">
@@ -8929,7 +8929,7 @@
         <v>Montgeron</v>
       </c>
       <c r="G340" t="str">
-        <v>421</v>
+        <v>91421</v>
       </c>
     </row>
     <row r="341">
@@ -8946,7 +8946,7 @@
         <v>Arpajon</v>
       </c>
       <c r="G341" t="str">
-        <v>021</v>
+        <v>91021</v>
       </c>
     </row>
     <row r="342">
@@ -8963,7 +8963,7 @@
         <v>Verrières-Le-Buisson</v>
       </c>
       <c r="G342" t="str">
-        <v>645</v>
+        <v>91645</v>
       </c>
     </row>
     <row r="343">
@@ -8980,7 +8980,7 @@
         <v>Suresnes</v>
       </c>
       <c r="G343" t="str">
-        <v>073</v>
+        <v>92073</v>
       </c>
     </row>
     <row r="344">
@@ -8997,7 +8997,7 @@
         <v>Rosny-sous-Bois</v>
       </c>
       <c r="G344" t="str">
-        <v>064</v>
+        <v>93064</v>
       </c>
     </row>
     <row r="345">
@@ -9014,7 +9014,7 @@
         <v>Livry-Gargan</v>
       </c>
       <c r="G345" t="str">
-        <v>046</v>
+        <v>93046</v>
       </c>
     </row>
     <row r="346">
@@ -9031,7 +9031,7 @@
         <v>Noisy-le-Grand</v>
       </c>
       <c r="G346" t="str">
-        <v>051</v>
+        <v>93051</v>
       </c>
     </row>
     <row r="347">
@@ -9048,7 +9048,7 @@
         <v>Sannois</v>
       </c>
       <c r="G347" t="str">
-        <v>582</v>
+        <v>95582</v>
       </c>
     </row>
     <row r="348">
@@ -9082,7 +9082,7 @@
         <v>Dourdan</v>
       </c>
       <c r="G349" t="str">
-        <v>200</v>
+        <v>91200</v>
       </c>
     </row>
     <row r="350">
@@ -9099,7 +9099,7 @@
         <v>Stains</v>
       </c>
       <c r="G350" t="str">
-        <v>072</v>
+        <v>93072</v>
       </c>
     </row>
     <row r="351">
@@ -9116,7 +9116,7 @@
         <v>Nogent-sur-Marne</v>
       </c>
       <c r="G351" t="str">
-        <v>052</v>
+        <v>94052</v>
       </c>
     </row>
     <row r="352">
@@ -9133,7 +9133,7 @@
         <v>Morsang-sur-Orge</v>
       </c>
       <c r="G352" t="str">
-        <v>434</v>
+        <v>91434</v>
       </c>
     </row>
     <row r="353">
@@ -9150,7 +9150,7 @@
         <v>Fontenay-aux-Roses</v>
       </c>
       <c r="G353" t="str">
-        <v>032</v>
+        <v>92032</v>
       </c>
     </row>
     <row r="354">
@@ -9167,7 +9167,7 @@
         <v>Villetaneuse</v>
       </c>
       <c r="G354" t="str">
-        <v>079</v>
+        <v>93079</v>
       </c>
     </row>
     <row r="355">
@@ -9184,7 +9184,7 @@
         <v>Villeneuve-Saint-Georges</v>
       </c>
       <c r="G355" t="str">
-        <v>078</v>
+        <v>94078</v>
       </c>
     </row>
     <row r="356">
@@ -9201,7 +9201,7 @@
         <v>Arcueil</v>
       </c>
       <c r="G356" t="str">
-        <v>003</v>
+        <v>94003</v>
       </c>
     </row>
     <row r="357">
@@ -9218,7 +9218,7 @@
         <v>Gennevilliers</v>
       </c>
       <c r="G357" t="str">
-        <v>036</v>
+        <v>92036</v>
       </c>
     </row>
     <row r="358">
@@ -9235,7 +9235,7 @@
         <v>Villejuif</v>
       </c>
       <c r="G358" t="str">
-        <v>076</v>
+        <v>94076</v>
       </c>
     </row>
     <row r="359">
@@ -9252,7 +9252,7 @@
         <v>Choisy-le-Roi</v>
       </c>
       <c r="G359" t="str">
-        <v>022</v>
+        <v>94022</v>
       </c>
     </row>
     <row r="360">
@@ -9269,7 +9269,7 @@
         <v>Trappes</v>
       </c>
       <c r="G360" t="str">
-        <v>621</v>
+        <v>78621</v>
       </c>
     </row>
     <row r="361">
@@ -9286,7 +9286,7 @@
         <v>Croissy-sur-Seine</v>
       </c>
       <c r="G361" t="str">
-        <v>190</v>
+        <v>78190</v>
       </c>
     </row>
     <row r="362">
@@ -9303,7 +9303,7 @@
         <v>Bondy</v>
       </c>
       <c r="G362" t="str">
-        <v>010</v>
+        <v>93010</v>
       </c>
     </row>
     <row r="363">
@@ -9320,7 +9320,7 @@
         <v>Lognes</v>
       </c>
       <c r="G363" t="str">
-        <v>258</v>
+        <v>77258</v>
       </c>
     </row>
     <row r="364">
@@ -9337,7 +9337,7 @@
         <v>Pontoise</v>
       </c>
       <c r="G364" t="str">
-        <v>500</v>
+        <v>95500</v>
       </c>
     </row>
     <row r="365">
@@ -9354,7 +9354,7 @@
         <v>Noisiel</v>
       </c>
       <c r="G365" t="str">
-        <v>337</v>
+        <v>77337</v>
       </c>
     </row>
     <row r="366">
@@ -9371,7 +9371,7 @@
         <v>Conflans-Sainte-Honorine</v>
       </c>
       <c r="G366" t="str">
-        <v>172</v>
+        <v>78172</v>
       </c>
     </row>
     <row r="367">
@@ -9388,7 +9388,7 @@
         <v>La Celle-Saint-Cloud</v>
       </c>
       <c r="G367" t="str">
-        <v>126</v>
+        <v>78126</v>
       </c>
     </row>
     <row r="368">
@@ -9405,7 +9405,7 @@
         <v>Villepreux</v>
       </c>
       <c r="G368" t="str">
-        <v>674</v>
+        <v>78674</v>
       </c>
     </row>
     <row r="369">
@@ -9422,7 +9422,7 @@
         <v>Orly</v>
       </c>
       <c r="G369" t="str">
-        <v>054</v>
+        <v>94054</v>
       </c>
     </row>
     <row r="370">
@@ -9439,7 +9439,7 @@
         <v>Deuil-la-Barre</v>
       </c>
       <c r="G370" t="str">
-        <v>197</v>
+        <v>95197</v>
       </c>
     </row>
     <row r="371">
@@ -9456,7 +9456,7 @@
         <v>Ermont</v>
       </c>
       <c r="G371" t="str">
-        <v>219</v>
+        <v>95219</v>
       </c>
     </row>
     <row r="372">
@@ -9473,7 +9473,7 @@
         <v>Charenton-le-Pont</v>
       </c>
       <c r="G372" t="str">
-        <v>018</v>
+        <v>94018</v>
       </c>
     </row>
     <row r="373">
@@ -9490,7 +9490,7 @@
         <v>Ormesson-sur-Marne</v>
       </c>
       <c r="G373" t="str">
-        <v>055</v>
+        <v>94055</v>
       </c>
     </row>
     <row r="374">
@@ -9507,7 +9507,7 @@
         <v>Chaville</v>
       </c>
       <c r="G374" t="str">
-        <v>022</v>
+        <v>92022</v>
       </c>
     </row>
     <row r="375">
@@ -9524,7 +9524,7 @@
         <v>Meudon</v>
       </c>
       <c r="G375" t="str">
-        <v>048</v>
+        <v>92048</v>
       </c>
     </row>
     <row r="376">
@@ -9541,7 +9541,7 @@
         <v>Rueil-Malmaison</v>
       </c>
       <c r="G376" t="str">
-        <v>063</v>
+        <v>92063</v>
       </c>
     </row>
     <row r="377">
@@ -9558,7 +9558,7 @@
         <v>Claye-Souilly</v>
       </c>
       <c r="G377" t="str">
-        <v>118</v>
+        <v>77118</v>
       </c>
     </row>
     <row r="378">
@@ -9575,7 +9575,7 @@
         <v>Villeparisis</v>
       </c>
       <c r="G378" t="str">
-        <v>514</v>
+        <v>77514</v>
       </c>
     </row>
     <row r="379">
@@ -9592,7 +9592,7 @@
         <v>Draveil</v>
       </c>
       <c r="G379" t="str">
-        <v>201</v>
+        <v>91201</v>
       </c>
     </row>
     <row r="380">
@@ -9609,7 +9609,7 @@
         <v>Montreuil</v>
       </c>
       <c r="G380" t="str">
-        <v>267</v>
+        <v>28267</v>
       </c>
     </row>
     <row r="381">
@@ -9626,7 +9626,7 @@
         <v>Alfortville</v>
       </c>
       <c r="G381" t="str">
-        <v>002</v>
+        <v>94002</v>
       </c>
     </row>
     <row r="382">
@@ -9677,7 +9677,7 @@
         <v>Vitry-sur-Seine</v>
       </c>
       <c r="G384" t="str">
-        <v>081</v>
+        <v>94081</v>
       </c>
     </row>
     <row r="385">
@@ -9694,7 +9694,7 @@
         <v>Les Mureaux</v>
       </c>
       <c r="G385" t="str">
-        <v>440</v>
+        <v>78440</v>
       </c>
     </row>
     <row r="386">
@@ -9711,7 +9711,7 @@
         <v>Sartrouville</v>
       </c>
       <c r="G386" t="str">
-        <v>586</v>
+        <v>78586</v>
       </c>
     </row>
     <row r="387">
@@ -9728,7 +9728,7 @@
         <v>Viroflay</v>
       </c>
       <c r="G387" t="str">
-        <v>686</v>
+        <v>78686</v>
       </c>
     </row>
     <row r="388">
@@ -9745,7 +9745,7 @@
         <v>Voisins-le-Bretonneux</v>
       </c>
       <c r="G388" t="str">
-        <v>688</v>
+        <v>78688</v>
       </c>
     </row>
     <row r="389">
@@ -9762,7 +9762,7 @@
         <v>Garches</v>
       </c>
       <c r="G389" t="str">
-        <v>033</v>
+        <v>92033</v>
       </c>
     </row>
     <row r="390">
@@ -9779,7 +9779,7 @@
         <v>Aubervilliers</v>
       </c>
       <c r="G390" t="str">
-        <v>001</v>
+        <v>93001</v>
       </c>
     </row>
     <row r="391">
@@ -9796,7 +9796,7 @@
         <v>Saint-Ouen-L'Aumône</v>
       </c>
       <c r="G391" t="str">
-        <v>572</v>
+        <v>95572</v>
       </c>
     </row>
     <row r="392">
@@ -9830,7 +9830,7 @@
         <v>Boulogne-Billancourt</v>
       </c>
       <c r="G393" t="str">
-        <v>012</v>
+        <v>92012</v>
       </c>
     </row>
     <row r="394">
@@ -9847,7 +9847,7 @@
         <v>Créteil</v>
       </c>
       <c r="G394" t="str">
-        <v>028</v>
+        <v>94028</v>
       </c>
     </row>
     <row r="395">
@@ -9864,7 +9864,7 @@
         <v>Orsay</v>
       </c>
       <c r="G395" t="str">
-        <v>471</v>
+        <v>91471</v>
       </c>
     </row>
     <row r="396">
@@ -9881,7 +9881,7 @@
         <v>Les Ulis</v>
       </c>
       <c r="G396" t="str">
-        <v>692</v>
+        <v>91692</v>
       </c>
     </row>
     <row r="397">
@@ -9898,7 +9898,7 @@
         <v>Poissy</v>
       </c>
       <c r="G397" t="str">
-        <v>498</v>
+        <v>78498</v>
       </c>
     </row>
     <row r="398">
@@ -9915,7 +9915,7 @@
         <v>Louvres</v>
       </c>
       <c r="G398" t="str">
-        <v>351</v>
+        <v>95351</v>
       </c>
     </row>
     <row r="399">
@@ -9932,7 +9932,7 @@
         <v>Goussainville</v>
       </c>
       <c r="G399" t="str">
-        <v>185</v>
+        <v>28185</v>
       </c>
     </row>
     <row r="400">
@@ -10162,7 +10162,7 @@
         <v>59130</v>
       </c>
       <c r="G412" t="str">
-        <v>328</v>
+        <v>59328</v>
       </c>
       <c r="H412">
         <v>0</v>
@@ -10197,7 +10197,7 @@
         <v>60000</v>
       </c>
       <c r="G413" t="str">
-        <v>057</v>
+        <v>60057</v>
       </c>
       <c r="H413">
         <v>0</v>
@@ -10235,7 +10235,7 @@
         <v>59300</v>
       </c>
       <c r="G414" t="str">
-        <v>606</v>
+        <v>59606</v>
       </c>
       <c r="H414">
         <v>0</v>
@@ -10264,7 +10264,7 @@
         <v>59100</v>
       </c>
       <c r="G415" t="str">
-        <v>512</v>
+        <v>59512</v>
       </c>
       <c r="H415">
         <v>0</v>
@@ -10293,7 +10293,7 @@
         <v>60200</v>
       </c>
       <c r="G416" t="str">
-        <v>159</v>
+        <v>60159</v>
       </c>
       <c r="H416">
         <v>0</v>
@@ -10322,7 +10322,7 @@
         <v>59400</v>
       </c>
       <c r="G417" t="str">
-        <v>122</v>
+        <v>59122</v>
       </c>
       <c r="H417">
         <v>0</v>
@@ -10351,7 +10351,7 @@
         <v>62510</v>
       </c>
       <c r="G418" t="str">
-        <v>015</v>
+        <v>11015</v>
       </c>
       <c r="H418">
         <v>0</v>
@@ -10380,7 +10380,7 @@
         <v>59290</v>
       </c>
       <c r="G419" t="str">
-        <v>646</v>
+        <v>59646</v>
       </c>
       <c r="H419">
         <v>0</v>
@@ -10409,7 +10409,7 @@
         <v>59000</v>
       </c>
       <c r="G420" t="str">
-        <v>350</v>
+        <v>59350</v>
       </c>
       <c r="H420">
         <v>0</v>
@@ -10438,7 +10438,7 @@
         <v>59140</v>
       </c>
       <c r="G421" t="str">
-        <v>183</v>
+        <v>59183</v>
       </c>
       <c r="H421">
         <v>0</v>
@@ -10467,7 +10467,7 @@
         <v>2300</v>
       </c>
       <c r="G422" t="str">
-        <v>173</v>
+        <v>02173</v>
       </c>
       <c r="H422">
         <v>0</v>
@@ -10496,7 +10496,7 @@
         <v>2200</v>
       </c>
       <c r="G423" t="str">
-        <v>722</v>
+        <v>02722</v>
       </c>
       <c r="H423">
         <v>0</v>
@@ -10525,7 +10525,7 @@
         <v>59150</v>
       </c>
       <c r="G424" t="str">
-        <v>650</v>
+        <v>59650</v>
       </c>
       <c r="H424">
         <v>0</v>
@@ -10554,7 +10554,7 @@
         <v>59500</v>
       </c>
       <c r="G425" t="str">
-        <v>178</v>
+        <v>59178</v>
       </c>
       <c r="H425">
         <v>0</v>
@@ -10583,7 +10583,7 @@
         <v>60180</v>
       </c>
       <c r="G426" t="str">
-        <v>463</v>
+        <v>60463</v>
       </c>
       <c r="H426">
         <v>0</v>
@@ -10612,7 +10612,7 @@
         <v>59910</v>
       </c>
       <c r="G427" t="str">
-        <v>090</v>
+        <v>59090</v>
       </c>
       <c r="H427">
         <v>0</v>
@@ -10641,7 +10641,7 @@
         <v>60400</v>
       </c>
       <c r="G428" t="str">
-        <v>471</v>
+        <v>60471</v>
       </c>
       <c r="H428">
         <v>0</v>
@@ -10670,7 +10670,7 @@
         <v>62310</v>
       </c>
       <c r="G429" t="str">
-        <v>612</v>
+        <v>60612</v>
       </c>
       <c r="H429">
         <v>0</v>
@@ -10699,7 +10699,7 @@
         <v>60160</v>
       </c>
       <c r="G430" t="str">
-        <v>414</v>
+        <v>60414</v>
       </c>
       <c r="H430">
         <v>0</v>
@@ -10728,7 +10728,7 @@
         <v>80000</v>
       </c>
       <c r="G431" t="str">
-        <v>021</v>
+        <v>80021</v>
       </c>
       <c r="H431">
         <v>0</v>
@@ -10757,7 +10757,7 @@
         <v>60100</v>
       </c>
       <c r="G432" t="str">
-        <v>175</v>
+        <v>60175</v>
       </c>
       <c r="H432">
         <v>0</v>
@@ -10786,7 +10786,7 @@
         <v>80100</v>
       </c>
       <c r="G433" t="str">
-        <v>001</v>
+        <v>80001</v>
       </c>
       <c r="H433">
         <v>0</v>
@@ -10815,7 +10815,7 @@
         <v>59250</v>
       </c>
       <c r="G434" t="str">
-        <v>279</v>
+        <v>59279</v>
       </c>
       <c r="H434">
         <v>0</v>
@@ -10873,7 +10873,7 @@
         <v>59700</v>
       </c>
       <c r="G436" t="str">
-        <v>378</v>
+        <v>59378</v>
       </c>
       <c r="H436">
         <v>0</v>
@@ -10931,7 +10931,7 @@
         <v>59139</v>
       </c>
       <c r="G438" t="str">
-        <v>648</v>
+        <v>59648</v>
       </c>
       <c r="H438">
         <v>0</v>
@@ -10960,7 +10960,7 @@
         <v>59115</v>
       </c>
       <c r="G439" t="str">
-        <v>339</v>
+        <v>59339</v>
       </c>
       <c r="H439">
         <v>0</v>
@@ -11018,7 +11018,7 @@
         <v>59350</v>
       </c>
       <c r="G441" t="str">
-        <v>527</v>
+        <v>59527</v>
       </c>
       <c r="H441">
         <v>0</v>
@@ -11047,7 +11047,7 @@
         <v>59170</v>
       </c>
       <c r="G442" t="str">
-        <v>163</v>
+        <v>59163</v>
       </c>
       <c r="H442">
         <v>0</v>
@@ -11076,7 +11076,7 @@
         <v>86000</v>
       </c>
       <c r="G443" t="str">
-        <v>194</v>
+        <v>86194</v>
       </c>
       <c r="H443">
         <v>0</v>
@@ -11105,7 +11105,7 @@
         <v>24300</v>
       </c>
       <c r="G444" t="str">
-        <v>311</v>
+        <v>24311</v>
       </c>
       <c r="H444">
         <v>0</v>
@@ -11134,7 +11134,7 @@
         <v>33000</v>
       </c>
       <c r="G445" t="str">
-        <v>063</v>
+        <v>33063</v>
       </c>
       <c r="H445">
         <v>0</v>
@@ -11163,7 +11163,7 @@
         <v>24000</v>
       </c>
       <c r="G446" t="str">
-        <v>322</v>
+        <v>24322</v>
       </c>
       <c r="H446">
         <v>0</v>
@@ -11221,7 +11221,7 @@
         <v>33185</v>
       </c>
       <c r="G448" t="str">
-        <v>200</v>
+        <v>33200</v>
       </c>
       <c r="H448">
         <v>0</v>
@@ -11250,7 +11250,7 @@
         <v>33610</v>
       </c>
       <c r="G449" t="str">
-        <v>122</v>
+        <v>33122</v>
       </c>
       <c r="H449">
         <v>0</v>
@@ -11279,7 +11279,7 @@
         <v>16100</v>
       </c>
       <c r="G450" t="str">
-        <v>102</v>
+        <v>16102</v>
       </c>
       <c r="H450">
         <v>0</v>
@@ -11308,7 +11308,7 @@
         <v>33130</v>
       </c>
       <c r="G451" t="str">
-        <v>039</v>
+        <v>33039</v>
       </c>
       <c r="H451">
         <v>0</v>
@@ -11337,7 +11337,7 @@
         <v>33290</v>
       </c>
       <c r="G452" t="str">
-        <v>056</v>
+        <v>32056</v>
       </c>
       <c r="H452">
         <v>0</v>
@@ -11366,7 +11366,7 @@
         <v>33110</v>
       </c>
       <c r="G453" t="str">
-        <v>069</v>
+        <v>33069</v>
       </c>
       <c r="H453">
         <v>0</v>
@@ -11395,7 +11395,7 @@
         <v>33320</v>
       </c>
       <c r="G454" t="str">
-        <v>162</v>
+        <v>33162</v>
       </c>
       <c r="H454">
         <v>0</v>
@@ -11424,7 +11424,7 @@
         <v>24100</v>
       </c>
       <c r="G455" t="str">
-        <v>037</v>
+        <v>24037</v>
       </c>
       <c r="H455">
         <v>0</v>
@@ -11453,7 +11453,7 @@
         <v>33700</v>
       </c>
       <c r="G456" t="str">
-        <v>216</v>
+        <v>16216</v>
       </c>
       <c r="H456">
         <v>0</v>
@@ -11482,7 +11482,7 @@
         <v>33270</v>
       </c>
       <c r="G457" t="str">
-        <v>160</v>
+        <v>17160</v>
       </c>
       <c r="H457">
         <v>0</v>
@@ -11540,7 +11540,7 @@
         <v>40100</v>
       </c>
       <c r="G459" t="str">
-        <v>088</v>
+        <v>40088</v>
       </c>
       <c r="H459">
         <v>0</v>
@@ -11569,7 +11569,7 @@
         <v>16000</v>
       </c>
       <c r="G460" t="str">
-        <v>015</v>
+        <v>16015</v>
       </c>
       <c r="H460">
         <v>0</v>
@@ -11598,7 +11598,7 @@
         <v>47000</v>
       </c>
       <c r="G461" t="str">
-        <v>001</v>
+        <v>47001</v>
       </c>
       <c r="H461">
         <v>0</v>
@@ -11627,7 +11627,7 @@
         <v>79000</v>
       </c>
       <c r="G462" t="str">
-        <v>191</v>
+        <v>79191</v>
       </c>
       <c r="H462">
         <v>0</v>
@@ -11656,7 +11656,7 @@
         <v>33120</v>
       </c>
       <c r="G463" t="str">
-        <v>009</v>
+        <v>33009</v>
       </c>
       <c r="H463">
         <v>0</v>
@@ -11685,7 +11685,7 @@
         <v>33380</v>
       </c>
       <c r="G464" t="str">
-        <v>284</v>
+        <v>33284</v>
       </c>
       <c r="H464">
         <v>0</v>
@@ -11714,7 +11714,7 @@
         <v>33520</v>
       </c>
       <c r="G465" t="str">
-        <v>075</v>
+        <v>33075</v>
       </c>
       <c r="H465">
         <v>0</v>
@@ -11743,7 +11743,7 @@
         <v>86180</v>
       </c>
       <c r="G466" t="str">
-        <v>123</v>
+        <v>21123</v>
       </c>
       <c r="H466">
         <v>0</v>
@@ -11772,7 +11772,7 @@
         <v>17200</v>
       </c>
       <c r="G467" t="str">
-        <v>306</v>
+        <v>17306</v>
       </c>
       <c r="H467">
         <v>0</v>
@@ -11801,7 +11801,7 @@
         <v>19100</v>
       </c>
       <c r="G468" t="str">
-        <v>031</v>
+        <v>19031</v>
       </c>
       <c r="H468">
         <v>0</v>
@@ -11830,7 +11830,7 @@
         <v>17000</v>
       </c>
       <c r="G469" t="str">
-        <v>300</v>
+        <v>17300</v>
       </c>
       <c r="H469">
         <v>0</v>
@@ -11859,7 +11859,7 @@
         <v>17100</v>
       </c>
       <c r="G470" t="str">
-        <v>415</v>
+        <v>17415</v>
       </c>
       <c r="H470">
         <v>0</v>
@@ -11917,7 +11917,7 @@
         <v>33850</v>
       </c>
       <c r="G472" t="str">
-        <v>238</v>
+        <v>33238</v>
       </c>
       <c r="H472">
         <v>0</v>
@@ -11946,7 +11946,7 @@
         <v>40280</v>
       </c>
       <c r="G473" t="str">
-        <v>652</v>
+        <v>14652</v>
       </c>
       <c r="H473">
         <v>0</v>
@@ -11975,7 +11975,7 @@
         <v>40220</v>
       </c>
       <c r="G474" t="str">
-        <v>312</v>
+        <v>40312</v>
       </c>
       <c r="H474">
         <v>0</v>
@@ -12004,7 +12004,7 @@
         <v>47520</v>
       </c>
       <c r="G475" t="str">
-        <v>296</v>
+        <v>38296</v>
       </c>
       <c r="H475">
         <v>0</v>
@@ -12033,7 +12033,7 @@
         <v>87000</v>
       </c>
       <c r="G476" t="str">
-        <v>085</v>
+        <v>87085</v>
       </c>
       <c r="H476">
         <v>0</v>
@@ -12062,7 +12062,7 @@
         <v>31320</v>
       </c>
       <c r="G477" t="str">
-        <v>113</v>
+        <v>31113</v>
       </c>
       <c r="H477">
         <v>0</v>
@@ -12091,7 +12091,7 @@
         <v>81370</v>
       </c>
       <c r="G478" t="str">
-        <v>271</v>
+        <v>81271</v>
       </c>
       <c r="H478">
         <v>0</v>
@@ -12120,7 +12120,7 @@
         <v>31520</v>
       </c>
       <c r="G479" t="str">
-        <v>446</v>
+        <v>31446</v>
       </c>
       <c r="H479">
         <v>0</v>
@@ -12149,7 +12149,7 @@
         <v>30200</v>
       </c>
       <c r="G480" t="str">
-        <v>028</v>
+        <v>30028</v>
       </c>
       <c r="H480">
         <v>0</v>
@@ -12178,7 +12178,7 @@
         <v>31650</v>
       </c>
       <c r="G481" t="str">
-        <v>506</v>
+        <v>31506</v>
       </c>
       <c r="H481">
         <v>0</v>
@@ -12207,7 +12207,7 @@
         <v>66000</v>
       </c>
       <c r="G482" t="str">
-        <v>136</v>
+        <v>66136</v>
       </c>
       <c r="H482">
         <v>0</v>
@@ -12236,7 +12236,7 @@
         <v>31830</v>
       </c>
       <c r="G483" t="str">
-        <v>424</v>
+        <v>31424</v>
       </c>
       <c r="H483">
         <v>0</v>
@@ -12265,7 +12265,7 @@
         <v>34170</v>
       </c>
       <c r="G484" t="str">
-        <v>057</v>
+        <v>34057</v>
       </c>
       <c r="H484">
         <v>0</v>
@@ -12294,7 +12294,7 @@
         <v>31600</v>
       </c>
       <c r="G485" t="str">
-        <v>395</v>
+        <v>31395</v>
       </c>
       <c r="H485">
         <v>0</v>
@@ -12323,7 +12323,7 @@
         <v>30130</v>
       </c>
       <c r="G486" t="str">
-        <v>202</v>
+        <v>30202</v>
       </c>
       <c r="H486">
         <v>0</v>
@@ -12352,7 +12352,7 @@
         <v>9000</v>
       </c>
       <c r="G487" t="str">
-        <v>122</v>
+        <v>09122</v>
       </c>
       <c r="H487">
         <v>0</v>
@@ -12381,7 +12381,7 @@
         <v>34500</v>
       </c>
       <c r="G488" t="str">
-        <v>032</v>
+        <v>34032</v>
       </c>
       <c r="H488">
         <v>0</v>
@@ -12410,7 +12410,7 @@
         <v>81300</v>
       </c>
       <c r="G489" t="str">
-        <v>105</v>
+        <v>81105</v>
       </c>
       <c r="H489">
         <v>0</v>
@@ -12439,7 +12439,7 @@
         <v>30100</v>
       </c>
       <c r="G490" t="str">
-        <v>007</v>
+        <v>30007</v>
       </c>
       <c r="H490">
         <v>0</v>
@@ -12468,7 +12468,7 @@
         <v>12000</v>
       </c>
       <c r="G491" t="str">
-        <v>202</v>
+        <v>12202</v>
       </c>
       <c r="H491">
         <v>0</v>
@@ -12497,7 +12497,7 @@
         <v>34400</v>
       </c>
       <c r="G492" t="str">
-        <v>145</v>
+        <v>34145</v>
       </c>
       <c r="H492">
         <v>0</v>
@@ -12526,7 +12526,7 @@
         <v>34110</v>
       </c>
       <c r="G493" t="str">
-        <v>108</v>
+        <v>34108</v>
       </c>
       <c r="H493">
         <v>0</v>
@@ -12555,7 +12555,7 @@
         <v>30300</v>
       </c>
       <c r="G494" t="str">
-        <v>032</v>
+        <v>30032</v>
       </c>
       <c r="H494">
         <v>0</v>
@@ -12584,7 +12584,7 @@
         <v>11100</v>
       </c>
       <c r="G495" t="str">
-        <v>262</v>
+        <v>11262</v>
       </c>
       <c r="H495">
         <v>0</v>
@@ -12642,7 +12642,7 @@
         <v>65100</v>
       </c>
       <c r="G497" t="str">
-        <v>286</v>
+        <v>65286</v>
       </c>
       <c r="H497">
         <v>0</v>
@@ -12671,7 +12671,7 @@
         <v>46100</v>
       </c>
       <c r="G498" t="str">
-        <v>102</v>
+        <v>46102</v>
       </c>
       <c r="H498">
         <v>0</v>
@@ -12700,7 +12700,7 @@
         <v>65000</v>
       </c>
       <c r="G499" t="str">
-        <v>440</v>
+        <v>65440</v>
       </c>
       <c r="H499">
         <v>0</v>
@@ -12729,7 +12729,7 @@
         <v>81000</v>
       </c>
       <c r="G500" t="str">
-        <v>004</v>
+        <v>81004</v>
       </c>
       <c r="H500">
         <v>0</v>
@@ -12787,7 +12787,7 @@
         <v>31770</v>
       </c>
       <c r="G502" t="str">
-        <v>149</v>
+        <v>31149</v>
       </c>
       <c r="H502">
         <v>0</v>
@@ -12816,7 +12816,7 @@
         <v>31000</v>
       </c>
       <c r="G503" t="str">
-        <v>555</v>
+        <v>31555</v>
       </c>
       <c r="H503">
         <v>0</v>
@@ -12845,7 +12845,7 @@
         <v>81400</v>
       </c>
       <c r="G504" t="str">
-        <v>060</v>
+        <v>81060</v>
       </c>
       <c r="H504">
         <v>0</v>
@@ -12874,7 +12874,7 @@
         <v>31130</v>
       </c>
       <c r="G505" t="str">
-        <v>044</v>
+        <v>31044</v>
       </c>
       <c r="H505">
         <v>0</v>
@@ -12903,7 +12903,7 @@
         <v>31270</v>
       </c>
       <c r="G506" t="str">
-        <v>157</v>
+        <v>31157</v>
       </c>
       <c r="H506">
         <v>0</v>
@@ -12932,7 +12932,7 @@
         <v>31270</v>
       </c>
       <c r="G507" t="str">
-        <v>203</v>
+        <v>31203</v>
       </c>
       <c r="H507">
         <v>0</v>
@@ -12990,7 +12990,7 @@
         <v>31120</v>
       </c>
       <c r="G509" t="str">
-        <v>433</v>
+        <v>31433</v>
       </c>
       <c r="H509">
         <v>0</v>
@@ -13019,7 +13019,7 @@
         <v>34430</v>
       </c>
       <c r="G510" t="str">
-        <v>270</v>
+        <v>34270</v>
       </c>
       <c r="H510">
         <v>0</v>
@@ -13048,7 +13048,7 @@
         <v>34470</v>
       </c>
       <c r="G511" t="str">
-        <v>198</v>
+        <v>34198</v>
       </c>
       <c r="H511">
         <v>0</v>
@@ -13077,7 +13077,7 @@
         <v>11000</v>
       </c>
       <c r="G512" t="str">
-        <v>069</v>
+        <v>11069</v>
       </c>
       <c r="H512">
         <v>0</v>
@@ -13106,7 +13106,7 @@
         <v>34970</v>
       </c>
       <c r="G513" t="str">
-        <v>129</v>
+        <v>34129</v>
       </c>
       <c r="H513">
         <v>0</v>
@@ -13135,7 +13135,7 @@
         <v>34200</v>
       </c>
       <c r="G514" t="str">
-        <v>301</v>
+        <v>34301</v>
       </c>
       <c r="H514">
         <v>0</v>
@@ -13164,7 +13164,7 @@
         <v>31170</v>
       </c>
       <c r="G515" t="str">
-        <v>557</v>
+        <v>31557</v>
       </c>
       <c r="H515">
         <v>0</v>
@@ -13193,7 +13193,7 @@
         <v>11300</v>
       </c>
       <c r="G516" t="str">
-        <v>206</v>
+        <v>11206</v>
       </c>
       <c r="H516">
         <v>0</v>
@@ -13222,7 +13222,7 @@
         <v>82000</v>
       </c>
       <c r="G517" t="str">
-        <v>121</v>
+        <v>82121</v>
       </c>
       <c r="H517">
         <v>0</v>
@@ -13251,7 +13251,7 @@
         <v>30000</v>
       </c>
       <c r="G518" t="str">
-        <v>189</v>
+        <v>30189</v>
       </c>
       <c r="H518">
         <v>0</v>
@@ -13280,7 +13280,7 @@
         <v>34000</v>
       </c>
       <c r="G519" t="str">
-        <v>172</v>
+        <v>34172</v>
       </c>
       <c r="H519">
         <v>0</v>
@@ -13309,7 +13309,7 @@
         <v>46100</v>
       </c>
       <c r="G520" t="str">
-        <v>102</v>
+        <v>46102</v>
       </c>
       <c r="H520">
         <v>0</v>
@@ -13338,7 +13338,7 @@
         <v>9100</v>
       </c>
       <c r="G521" t="str">
-        <v>225</v>
+        <v>09225</v>
       </c>
       <c r="H521">
         <v>0</v>
@@ -13367,7 +13367,7 @@
         <v>12200</v>
       </c>
       <c r="G522" t="str">
-        <v>300</v>
+        <v>12300</v>
       </c>
       <c r="H522">
         <v>0</v>
@@ -13396,7 +13396,7 @@
         <v>32100</v>
       </c>
       <c r="G523" t="str">
-        <v>107</v>
+        <v>32107</v>
       </c>
       <c r="H523">
         <v>0</v>
@@ -13425,7 +13425,7 @@
         <v>32000</v>
       </c>
       <c r="G524" t="str">
-        <v>013</v>
+        <v>32013</v>
       </c>
       <c r="H524">
         <v>0</v>
@@ -13454,7 +13454,7 @@
         <v>46000</v>
       </c>
       <c r="G525" t="str">
-        <v>042</v>
+        <v>46042</v>
       </c>
       <c r="H525">
         <v>0</v>
@@ -13483,7 +13483,7 @@
         <v>81600</v>
       </c>
       <c r="G526" t="str">
-        <v>099</v>
+        <v>81099</v>
       </c>
       <c r="H526">
         <v>0</v>
@@ -13512,7 +13512,7 @@
         <v>65000</v>
       </c>
       <c r="G527" t="str">
-        <v>440</v>
+        <v>65440</v>
       </c>
       <c r="H527">
         <v>0</v>
@@ -13541,7 +13541,7 @@
         <v>83330</v>
       </c>
       <c r="G528" t="str">
-        <v>016</v>
+        <v>83016</v>
       </c>
       <c r="H528">
         <v>0</v>
@@ -13570,7 +13570,7 @@
         <v>83170</v>
       </c>
       <c r="G529" t="str">
-        <v>023</v>
+        <v>83023</v>
       </c>
       <c r="H529">
         <v>0</v>
@@ -13599,7 +13599,7 @@
         <v>6110</v>
       </c>
       <c r="G530" t="str">
-        <v>030</v>
+        <v>06030</v>
       </c>
       <c r="H530">
         <v>0</v>
@@ -13628,7 +13628,7 @@
         <v>83470</v>
       </c>
       <c r="G531" t="str">
-        <v>116</v>
+        <v>83116</v>
       </c>
       <c r="H531">
         <v>0</v>
@@ -13657,7 +13657,7 @@
         <v>83390</v>
       </c>
       <c r="G532" t="str">
-        <v>049</v>
+        <v>83049</v>
       </c>
       <c r="H532">
         <v>0</v>
@@ -13686,7 +13686,7 @@
         <v>84300</v>
       </c>
       <c r="G533" t="str">
-        <v>035</v>
+        <v>84035</v>
       </c>
       <c r="H533">
         <v>0</v>
@@ -13715,7 +13715,7 @@
         <v>83270</v>
       </c>
       <c r="G534" t="str">
-        <v>112</v>
+        <v>83112</v>
       </c>
       <c r="H534">
         <v>0</v>
@@ -13744,7 +13744,7 @@
         <v>83000</v>
       </c>
       <c r="G535" t="str">
-        <v>137</v>
+        <v>83137</v>
       </c>
       <c r="H535">
         <v>0</v>
@@ -13773,7 +13773,7 @@
         <v>13080</v>
       </c>
       <c r="G536" t="str">
-        <v>001</v>
+        <v>13001</v>
       </c>
       <c r="H536">
         <v>0</v>
@@ -13808,7 +13808,7 @@
         <v>13104</v>
       </c>
       <c r="G537" t="str">
-        <v>004</v>
+        <v>13004</v>
       </c>
       <c r="H537">
         <v>0</v>
@@ -13837,7 +13837,7 @@
         <v>83130</v>
       </c>
       <c r="G538" t="str">
-        <v>092</v>
+        <v>04092</v>
       </c>
       <c r="H538">
         <v>0</v>
@@ -13866,7 +13866,7 @@
         <v>13410</v>
       </c>
       <c r="G539" t="str">
-        <v>050</v>
+        <v>13050</v>
       </c>
       <c r="H539">
         <v>0</v>
@@ -13895,7 +13895,7 @@
         <v>4000</v>
       </c>
       <c r="G540" t="str">
-        <v>070</v>
+        <v>04070</v>
       </c>
       <c r="H540">
         <v>0</v>
@@ -13924,7 +13924,7 @@
         <v>4100</v>
       </c>
       <c r="G541" t="str">
-        <v>112</v>
+        <v>04112</v>
       </c>
       <c r="H541">
         <v>0</v>
@@ -13953,7 +13953,7 @@
         <v>13400</v>
       </c>
       <c r="G542" t="str">
-        <v>005</v>
+        <v>13005</v>
       </c>
       <c r="H542">
         <v>0</v>
@@ -13982,7 +13982,7 @@
         <v>13117</v>
       </c>
       <c r="G543" t="str">
-        <v>056</v>
+        <v>13056</v>
       </c>
       <c r="H543">
         <v>0</v>
@@ -14011,7 +14011,7 @@
         <v>83700</v>
       </c>
       <c r="G544" t="str">
-        <v>493</v>
+        <v>24493</v>
       </c>
       <c r="H544">
         <v>0</v>
@@ -14040,7 +14040,7 @@
         <v>83520</v>
       </c>
       <c r="G545" t="str">
-        <v>107</v>
+        <v>83107</v>
       </c>
       <c r="H545">
         <v>0</v>
@@ -14069,7 +14069,7 @@
         <v>13800</v>
       </c>
       <c r="G546" t="str">
-        <v>047</v>
+        <v>13047</v>
       </c>
       <c r="H546">
         <v>0</v>
@@ -14098,7 +14098,7 @@
         <v>6220</v>
       </c>
       <c r="G547" t="str">
-        <v>155</v>
+        <v>06155</v>
       </c>
       <c r="H547">
         <v>0</v>
@@ -14185,7 +14185,7 @@
         <v>83400</v>
       </c>
       <c r="G550" t="str">
-        <v>069</v>
+        <v>83069</v>
       </c>
       <c r="H550">
         <v>0</v>
@@ -14214,7 +14214,7 @@
         <v>6600</v>
       </c>
       <c r="G551" t="str">
-        <v>004</v>
+        <v>06004</v>
       </c>
       <c r="H551">
         <v>0</v>
@@ -14243,7 +14243,7 @@
         <v>13400</v>
       </c>
       <c r="G552" t="str">
-        <v>005</v>
+        <v>13005</v>
       </c>
       <c r="H552">
         <v>0</v>
@@ -14272,7 +14272,7 @@
         <v>13117</v>
       </c>
       <c r="G553" t="str">
-        <v>056</v>
+        <v>13056</v>
       </c>
       <c r="H553">
         <v>0</v>
@@ -14301,7 +14301,7 @@
         <v>83320</v>
       </c>
       <c r="G554" t="str">
-        <v>034</v>
+        <v>83034</v>
       </c>
       <c r="H554">
         <v>0</v>
@@ -14330,7 +14330,7 @@
         <v>84250</v>
       </c>
       <c r="G555" t="str">
-        <v>132</v>
+        <v>84132</v>
       </c>
       <c r="H555">
         <v>0</v>
@@ -14359,7 +14359,7 @@
         <v>84400</v>
       </c>
       <c r="G556" t="str">
-        <v>003</v>
+        <v>84003</v>
       </c>
       <c r="H556">
         <v>0</v>
@@ -14388,7 +14388,7 @@
         <v>84000</v>
       </c>
       <c r="G557" t="str">
-        <v>007</v>
+        <v>84007</v>
       </c>
       <c r="H557">
         <v>0</v>
@@ -14417,7 +14417,7 @@
         <v>13210</v>
       </c>
       <c r="G558" t="str">
-        <v>100</v>
+        <v>13100</v>
       </c>
       <c r="H558">
         <v>0</v>
@@ -14481,7 +14481,7 @@
         <v>83600</v>
       </c>
       <c r="G560" t="str">
-        <v>061</v>
+        <v>83061</v>
       </c>
       <c r="H560">
         <v>0</v>
@@ -14510,7 +14510,7 @@
         <v>84100</v>
       </c>
       <c r="G561" t="str">
-        <v>087</v>
+        <v>84087</v>
       </c>
       <c r="H561">
         <v>0</v>
@@ -14539,7 +14539,7 @@
         <v>13530</v>
       </c>
       <c r="G562" t="str">
-        <v>110</v>
+        <v>13110</v>
       </c>
       <c r="H562">
         <v>0</v>
@@ -14568,7 +14568,7 @@
         <v>83220</v>
       </c>
       <c r="G563" t="str">
-        <v>098</v>
+        <v>83098</v>
       </c>
       <c r="H563">
         <v>0</v>
@@ -14597,7 +14597,7 @@
         <v>5100</v>
       </c>
       <c r="G564" t="str">
-        <v>023</v>
+        <v>05023</v>
       </c>
       <c r="H564">
         <v>0</v>
@@ -14626,7 +14626,7 @@
         <v>27170</v>
       </c>
       <c r="G565" t="str">
-        <v>051</v>
+        <v>27051</v>
       </c>
       <c r="H565" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14655,7 +14655,7 @@
         <v>27160</v>
       </c>
       <c r="G566" t="str">
-        <v>112</v>
+        <v>27112</v>
       </c>
       <c r="H566" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14684,7 +14684,7 @@
         <v>27600</v>
       </c>
       <c r="G567" t="str">
-        <v>275</v>
+        <v>27275</v>
       </c>
       <c r="H567" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14713,7 +14713,7 @@
         <v>27140</v>
       </c>
       <c r="G568" t="str">
-        <v>284</v>
+        <v>27284</v>
       </c>
       <c r="H568" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14742,7 +14742,7 @@
         <v>27480</v>
       </c>
       <c r="G569" t="str">
-        <v>377</v>
+        <v>27377</v>
       </c>
       <c r="H569" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14771,7 +14771,7 @@
         <v>27160</v>
       </c>
       <c r="G570" t="str">
-        <v>198</v>
+        <v>27198</v>
       </c>
       <c r="H570" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14800,7 +14800,7 @@
         <v>27120</v>
       </c>
       <c r="G571" t="str">
-        <v>448</v>
+        <v>27448</v>
       </c>
       <c r="H571" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14829,7 +14829,7 @@
         <v>27250</v>
       </c>
       <c r="G572" t="str">
-        <v>502</v>
+        <v>27502</v>
       </c>
       <c r="H572" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>
@@ -14858,7 +14858,7 @@
         <v>27420</v>
       </c>
       <c r="G573" t="str">
-        <v>213</v>
+        <v>27213</v>
       </c>
       <c r="H573" t="str">
         <v>https://www.paris-normandie.fr/actualites/politique/a-bernay-quel-candidat-soutiendra-le-mouvement-de-sebastien-lecornu-ensemble-pour-l-eure-HH16226919#.XiFx3gnvdKs.twitter</v>

</xml_diff>